<commit_message>
fix error in FET thermal calcs
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Component_Selection.xlsx
+++ b/00_PROJECT_RESEARCH/Component_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1EC3B-C76C-441A-A174-4CFA719CEE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F5BC22-31F4-425E-8342-085A2FE62B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
+    <workbookView xWindow="-30828" yWindow="12060" windowWidth="30936" windowHeight="16776" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Info" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,37 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -721,15 +751,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>3976</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>314875</xdr:colOff>
+      <xdr:colOff>1046922</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>104367</xdr:rowOff>
+      <xdr:rowOff>183880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -752,8 +782,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30480" y="403860"/>
-          <a:ext cx="3246398" cy="1163547"/>
+          <a:off x="3976" y="213634"/>
+          <a:ext cx="4011433" cy="1454489"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,54 +1213,55 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A6DD2-EC01-41A2-B284-C1859DA82837}">
-  <dimension ref="N1:N6"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="112.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="14:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N1" s="20" t="s">
+    <row r="1" spans="1:1" ht="216" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N2" s="8" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N3" s="8" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N4" s="8" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N5" s="8" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N6" s="8" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" xr:uid="{31B67733-6B22-4721-B151-5A3BE1AD06D4}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{C8A36AFB-B0B7-4064-8F12-2DCAD0245A94}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{0D71EA45-6825-4A58-83B7-78D468C0684B}"/>
-    <hyperlink ref="N5" r:id="rId4" xr:uid="{4BD38861-BF3A-42A4-9F4A-2CD1EA611117}"/>
-    <hyperlink ref="N6" r:id="rId5" xr:uid="{57F66591-D2A1-4114-9E2A-3BD9EA83CCB8}"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{57F66591-D2A1-4114-9E2A-3BD9EA83CCB8}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{4BD38861-BF3A-42A4-9F4A-2CD1EA611117}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{0D71EA45-6825-4A58-83B7-78D468C0684B}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{C8A36AFB-B0B7-4064-8F12-2DCAD0245A94}"/>
+    <hyperlink ref="A3" r:id="rId5" xr:uid="{31B67733-6B22-4721-B151-5A3BE1AD06D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -1280,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44782264-4582-4BFB-8AD9-CCF220720B86}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1369,15 +1400,15 @@
         <v>1</v>
       </c>
       <c r="B19" s="38">
-        <f>ROUND($B$11+$B$15*$B$13*$B$13*($B$12/$A19),2)</f>
+        <f>ROUND($B$11+$B$15*($B$13/$A19)*($B$13/$A19)*($B$12),2)</f>
         <v>101.6</v>
       </c>
       <c r="C19" s="38">
-        <f>ROUND($B$11+$B$14*$B$13*$B$13*($B$12/$A19),2)</f>
+        <f>ROUND($B$11+$B$14*($B$13/$A19)*($B$13/$A19)*($B$12),2)</f>
         <v>1100</v>
       </c>
       <c r="D19" s="38">
-        <f>ROUND($B$11+$B$16*$B$13*$B$13*($B$12/$A19),2)</f>
+        <f>ROUND($B$11+$B$16*($B$13/$A19)*($B$13/$A19)*($B$12),2)</f>
         <v>2660</v>
       </c>
     </row>
@@ -1386,16 +1417,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="38">
-        <f t="shared" ref="B20:B38" si="0">ROUND($B$11+0.8*$B$13*$B$13*($B$12/A20),2)</f>
-        <v>80.8</v>
+        <f t="shared" ref="B20:B38" si="0">ROUND($B$11+$B$15*($B$13/$A20)*($B$13/$A20)*($B$12),2)</f>
+        <v>70.400000000000006</v>
       </c>
       <c r="C20" s="38">
-        <f t="shared" ref="C20:C38" si="1">ROUND($B$11+$B$14*$B$13*$B$13*($B$12/$A20),2)</f>
-        <v>580</v>
+        <f t="shared" ref="C20:C38" si="1">ROUND($B$11+$B$14*($B$13/$A20)*($B$13/$A20)*($B$12),2)</f>
+        <v>320</v>
       </c>
       <c r="D20" s="38">
-        <f t="shared" ref="D20:D38" si="2">ROUND($B$11+$B$16*$B$13*$B$13*($B$12/$A20),2)</f>
-        <v>1360</v>
+        <f t="shared" ref="D20:D38" si="2">ROUND($B$11+$B$16*($B$13/$A20)*($B$13/$A20)*($B$12),2)</f>
+        <v>710</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1404,15 +1435,15 @@
       </c>
       <c r="B21" s="38">
         <f t="shared" si="0"/>
-        <v>73.87</v>
+        <v>64.62</v>
       </c>
       <c r="C21" s="38">
         <f t="shared" si="1"/>
-        <v>406.67</v>
+        <v>175.56</v>
       </c>
       <c r="D21" s="38">
         <f t="shared" si="2"/>
-        <v>926.67</v>
+        <v>348.89</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1421,15 +1452,15 @@
       </c>
       <c r="B22" s="38">
         <f t="shared" si="0"/>
-        <v>70.400000000000006</v>
+        <v>62.6</v>
       </c>
       <c r="C22" s="38">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>125</v>
       </c>
       <c r="D22" s="38">
         <f t="shared" si="2"/>
-        <v>710</v>
+        <v>222.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1438,15 +1469,15 @@
       </c>
       <c r="B23" s="38">
         <f t="shared" si="0"/>
-        <v>68.319999999999993</v>
+        <v>61.66</v>
       </c>
       <c r="C23" s="38">
         <f t="shared" si="1"/>
-        <v>268</v>
+        <v>101.6</v>
       </c>
       <c r="D23" s="38">
         <f t="shared" si="2"/>
-        <v>580</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1455,15 +1486,15 @@
       </c>
       <c r="B24" s="38">
         <f t="shared" si="0"/>
-        <v>66.930000000000007</v>
+        <v>61.16</v>
       </c>
       <c r="C24" s="38">
         <f t="shared" si="1"/>
-        <v>233.33</v>
+        <v>88.89</v>
       </c>
       <c r="D24" s="38">
         <f t="shared" si="2"/>
-        <v>493.33</v>
+        <v>132.22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1472,15 +1503,15 @@
       </c>
       <c r="B25" s="38">
         <f t="shared" si="0"/>
-        <v>65.94</v>
+        <v>60.85</v>
       </c>
       <c r="C25" s="38">
         <f t="shared" si="1"/>
-        <v>208.57</v>
+        <v>81.22</v>
       </c>
       <c r="D25" s="38">
         <f t="shared" si="2"/>
-        <v>431.43</v>
+        <v>113.06</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1489,15 +1520,15 @@
       </c>
       <c r="B26" s="38">
         <f t="shared" si="0"/>
-        <v>65.2</v>
+        <v>60.65</v>
       </c>
       <c r="C26" s="38">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>76.25</v>
       </c>
       <c r="D26" s="38">
         <f t="shared" si="2"/>
-        <v>385</v>
+        <v>100.63</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1506,15 +1537,15 @@
       </c>
       <c r="B27" s="38">
         <f t="shared" si="0"/>
-        <v>64.62</v>
+        <v>60.51</v>
       </c>
       <c r="C27" s="38">
         <f t="shared" si="1"/>
-        <v>175.56</v>
+        <v>72.84</v>
       </c>
       <c r="D27" s="38">
         <f t="shared" si="2"/>
-        <v>348.89</v>
+        <v>92.1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1523,15 +1554,15 @@
       </c>
       <c r="B28" s="38">
         <f t="shared" si="0"/>
-        <v>64.16</v>
+        <v>60.42</v>
       </c>
       <c r="C28" s="38">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="D28" s="38">
         <f t="shared" si="2"/>
-        <v>320</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1540,15 +1571,15 @@
       </c>
       <c r="B29" s="38">
         <f t="shared" si="0"/>
-        <v>63.78</v>
+        <v>60.34</v>
       </c>
       <c r="C29" s="38">
         <f t="shared" si="1"/>
-        <v>154.55000000000001</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="D29" s="38">
         <f t="shared" si="2"/>
-        <v>296.36</v>
+        <v>81.489999999999995</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1557,15 +1588,15 @@
       </c>
       <c r="B30" s="38">
         <f t="shared" si="0"/>
-        <v>63.47</v>
+        <v>60.29</v>
       </c>
       <c r="C30" s="38">
         <f t="shared" si="1"/>
-        <v>146.66999999999999</v>
+        <v>67.22</v>
       </c>
       <c r="D30" s="38">
         <f t="shared" si="2"/>
-        <v>276.67</v>
+        <v>78.06</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1574,15 +1605,15 @@
       </c>
       <c r="B31" s="38">
         <f t="shared" si="0"/>
-        <v>63.2</v>
+        <v>60.25</v>
       </c>
       <c r="C31" s="38">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>66.150000000000006</v>
       </c>
       <c r="D31" s="38">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>75.38</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1591,15 +1622,15 @@
       </c>
       <c r="B32" s="38">
         <f t="shared" si="0"/>
-        <v>62.97</v>
+        <v>60.21</v>
       </c>
       <c r="C32" s="38">
         <f t="shared" si="1"/>
-        <v>134.29</v>
+        <v>65.31</v>
       </c>
       <c r="D32" s="38">
         <f t="shared" si="2"/>
-        <v>245.71</v>
+        <v>73.27</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1608,15 +1639,15 @@
       </c>
       <c r="B33" s="38">
         <f t="shared" si="0"/>
-        <v>62.77</v>
+        <v>60.18</v>
       </c>
       <c r="C33" s="38">
         <f t="shared" si="1"/>
-        <v>129.33000000000001</v>
+        <v>64.62</v>
       </c>
       <c r="D33" s="38">
         <f t="shared" si="2"/>
-        <v>233.33</v>
+        <v>71.56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1625,15 +1656,15 @@
       </c>
       <c r="B34" s="38">
         <f t="shared" si="0"/>
-        <v>62.6</v>
+        <v>60.16</v>
       </c>
       <c r="C34" s="38">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>64.06</v>
       </c>
       <c r="D34" s="38">
         <f t="shared" si="2"/>
-        <v>222.5</v>
+        <v>70.16</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1642,15 +1673,15 @@
       </c>
       <c r="B35" s="38">
         <f t="shared" si="0"/>
-        <v>62.45</v>
+        <v>60.14</v>
       </c>
       <c r="C35" s="38">
         <f t="shared" si="1"/>
-        <v>121.18</v>
+        <v>63.6</v>
       </c>
       <c r="D35" s="38">
         <f t="shared" si="2"/>
-        <v>212.94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,15 +1690,15 @@
       </c>
       <c r="B36" s="38">
         <f t="shared" si="0"/>
-        <v>62.31</v>
+        <v>60.13</v>
       </c>
       <c r="C36" s="38">
         <f t="shared" si="1"/>
-        <v>117.78</v>
+        <v>63.21</v>
       </c>
       <c r="D36" s="38">
         <f t="shared" si="2"/>
-        <v>204.44</v>
+        <v>68.02</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1676,15 +1707,15 @@
       </c>
       <c r="B37" s="38">
         <f t="shared" si="0"/>
-        <v>62.19</v>
+        <v>60.12</v>
       </c>
       <c r="C37" s="38">
         <f t="shared" si="1"/>
-        <v>114.74</v>
+        <v>62.88</v>
       </c>
       <c r="D37" s="38">
         <f t="shared" si="2"/>
-        <v>196.84</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1693,28 +1724,38 @@
       </c>
       <c r="B38" s="38">
         <f t="shared" si="0"/>
-        <v>62.08</v>
+        <v>60.1</v>
       </c>
       <c r="C38" s="38">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>62.6</v>
       </c>
       <c r="D38" s="38">
         <f t="shared" si="2"/>
-        <v>190</v>
+        <v>66.5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B19:D38">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>120</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>120</formula>
       <formula>170</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>170</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2084,7 +2125,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated with lib components, adjusted board shape
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Component_Selection.xlsx
+++ b/00_PROJECT_RESEARCH/Component_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F5BC22-31F4-425E-8342-085A2FE62B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CB4E7-81DA-417D-9B6C-4F6958B1895A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="12060" windowWidth="30936" windowHeight="16776" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Info" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -673,66 +673,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -757,9 +697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1046922</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>183880</xdr:rowOff>
+      <xdr:colOff>1044382</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1098,15 +1038,15 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
@@ -1129,7 +1069,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
@@ -1148,7 +1088,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1107,7 @@
         <v>20.83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>8</v>
       </c>
@@ -1219,38 +1159,38 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="112.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="112.08984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="216" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>72</v>
       </c>
@@ -1276,13 +1216,13 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1309,434 +1249,444 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44782264-4582-4BFB-8AD9-CCF220720B86}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>87</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>88</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>89</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>90</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>91</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B19" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C19" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D19" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="38">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="38">
         <v>1</v>
       </c>
-      <c r="B19" s="38">
-        <f>ROUND($B$11+$B$15*($B$13/$A19)*($B$13/$A19)*($B$12),2)</f>
+      <c r="B20" s="38">
+        <f>ROUND($B$12+$B$16*($B$14/$A20)*($B$14/$A20)*($B$13),2)</f>
         <v>101.6</v>
       </c>
-      <c r="C19" s="38">
-        <f>ROUND($B$11+$B$14*($B$13/$A19)*($B$13/$A19)*($B$12),2)</f>
+      <c r="C20" s="38">
+        <f>ROUND($B$12+$B$15*($B$14/$A20)*($B$14/$A20)*($B$13),2)</f>
         <v>1100</v>
       </c>
-      <c r="D19" s="38">
-        <f>ROUND($B$11+$B$16*($B$13/$A19)*($B$13/$A19)*($B$12),2)</f>
+      <c r="D20" s="38">
+        <f>ROUND($B$12+$B$17*($B$14/$A20)*($B$14/$A20)*($B$13),2)</f>
         <v>2660</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="38">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="38">
         <v>2</v>
       </c>
-      <c r="B20" s="38">
-        <f t="shared" ref="B20:B38" si="0">ROUND($B$11+$B$15*($B$13/$A20)*($B$13/$A20)*($B$12),2)</f>
+      <c r="B21" s="38">
+        <f t="shared" ref="B21:B39" si="0">ROUND($B$12+$B$16*($B$14/$A21)*($B$14/$A21)*($B$13),2)</f>
         <v>70.400000000000006</v>
       </c>
-      <c r="C20" s="38">
-        <f t="shared" ref="C20:C38" si="1">ROUND($B$11+$B$14*($B$13/$A20)*($B$13/$A20)*($B$12),2)</f>
+      <c r="C21" s="38">
+        <f t="shared" ref="C21:C39" si="1">ROUND($B$12+$B$15*($B$14/$A21)*($B$14/$A21)*($B$13),2)</f>
         <v>320</v>
       </c>
-      <c r="D20" s="38">
-        <f t="shared" ref="D20:D38" si="2">ROUND($B$11+$B$16*($B$13/$A20)*($B$13/$A20)*($B$12),2)</f>
+      <c r="D21" s="38">
+        <f t="shared" ref="D21:D39" si="2">ROUND($B$12+$B$17*($B$14/$A21)*($B$14/$A21)*($B$13),2)</f>
         <v>710</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="38">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="38">
         <v>3</v>
       </c>
-      <c r="B21" s="38">
+      <c r="B22" s="38">
         <f t="shared" si="0"/>
         <v>64.62</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C22" s="38">
         <f t="shared" si="1"/>
         <v>175.56</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D22" s="38">
         <f t="shared" si="2"/>
         <v>348.89</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="38">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="38">
         <v>4</v>
       </c>
-      <c r="B22" s="38">
+      <c r="B23" s="38">
         <f t="shared" si="0"/>
         <v>62.6</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C23" s="38">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D23" s="38">
         <f t="shared" si="2"/>
         <v>222.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="38">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="38">
         <v>5</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B24" s="38">
         <f t="shared" si="0"/>
         <v>61.66</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C24" s="38">
         <f t="shared" si="1"/>
         <v>101.6</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D24" s="38">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="38">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="38">
         <v>6</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B25" s="38">
         <f t="shared" si="0"/>
         <v>61.16</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C25" s="38">
         <f t="shared" si="1"/>
         <v>88.89</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D25" s="38">
         <f t="shared" si="2"/>
         <v>132.22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="38">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="38">
         <v>7</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B26" s="38">
         <f t="shared" si="0"/>
         <v>60.85</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C26" s="38">
         <f t="shared" si="1"/>
         <v>81.22</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D26" s="38">
         <f t="shared" si="2"/>
         <v>113.06</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="38">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="38">
         <v>8</v>
       </c>
-      <c r="B26" s="38">
+      <c r="B27" s="38">
         <f t="shared" si="0"/>
         <v>60.65</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C27" s="38">
         <f t="shared" si="1"/>
         <v>76.25</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D27" s="38">
         <f t="shared" si="2"/>
         <v>100.63</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="38">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="38">
         <v>9</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B28" s="38">
         <f t="shared" si="0"/>
         <v>60.51</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C28" s="38">
         <f t="shared" si="1"/>
         <v>72.84</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D28" s="38">
         <f t="shared" si="2"/>
         <v>92.1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="38">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="38">
         <v>10</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B29" s="38">
         <f t="shared" si="0"/>
         <v>60.42</v>
       </c>
-      <c r="C28" s="38">
+      <c r="C29" s="38">
         <f t="shared" si="1"/>
         <v>70.400000000000006</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D29" s="38">
         <f t="shared" si="2"/>
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="38">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="38">
         <v>11</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B30" s="38">
         <f t="shared" si="0"/>
         <v>60.34</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C30" s="38">
         <f t="shared" si="1"/>
         <v>68.599999999999994</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D30" s="38">
         <f t="shared" si="2"/>
         <v>81.489999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="38">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="38">
         <v>12</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B31" s="38">
         <f t="shared" si="0"/>
         <v>60.29</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C31" s="38">
         <f t="shared" si="1"/>
         <v>67.22</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D31" s="38">
         <f t="shared" si="2"/>
         <v>78.06</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="38">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="38">
         <v>13</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B32" s="38">
         <f t="shared" si="0"/>
         <v>60.25</v>
       </c>
-      <c r="C31" s="38">
+      <c r="C32" s="38">
         <f t="shared" si="1"/>
         <v>66.150000000000006</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D32" s="38">
         <f t="shared" si="2"/>
         <v>75.38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="38">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="38">
         <v>14</v>
       </c>
-      <c r="B32" s="38">
+      <c r="B33" s="38">
         <f t="shared" si="0"/>
         <v>60.21</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C33" s="38">
         <f t="shared" si="1"/>
         <v>65.31</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D33" s="38">
         <f t="shared" si="2"/>
         <v>73.27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="38">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="38">
         <v>15</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B34" s="38">
         <f t="shared" si="0"/>
         <v>60.18</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C34" s="38">
         <f t="shared" si="1"/>
         <v>64.62</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D34" s="38">
         <f t="shared" si="2"/>
         <v>71.56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="38">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="38">
         <v>16</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B35" s="38">
         <f t="shared" si="0"/>
         <v>60.16</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C35" s="38">
         <f t="shared" si="1"/>
         <v>64.06</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D35" s="38">
         <f t="shared" si="2"/>
         <v>70.16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="38">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="38">
         <v>17</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B36" s="38">
         <f t="shared" si="0"/>
         <v>60.14</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C36" s="38">
         <f t="shared" si="1"/>
         <v>63.6</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D36" s="38">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="38">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="38">
         <v>18</v>
       </c>
-      <c r="B36" s="38">
+      <c r="B37" s="38">
         <f t="shared" si="0"/>
         <v>60.13</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C37" s="38">
         <f t="shared" si="1"/>
         <v>63.21</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D37" s="38">
         <f t="shared" si="2"/>
         <v>68.02</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="38">
         <v>19</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B38" s="38">
         <f t="shared" si="0"/>
         <v>60.12</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C38" s="38">
         <f t="shared" si="1"/>
         <v>62.88</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D38" s="38">
         <f t="shared" si="2"/>
         <v>67.2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="38">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="38">
         <v>20</v>
       </c>
-      <c r="B38" s="38">
+      <c r="B39" s="38">
         <f t="shared" si="0"/>
         <v>60.1</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C39" s="38">
         <f t="shared" si="1"/>
         <v>62.6</v>
       </c>
-      <c r="D38" s="38">
+      <c r="D39" s="38">
         <f t="shared" si="2"/>
         <v>66.5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B19:D38">
+  <conditionalFormatting sqref="B20:D39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>120</formula>
     </cfRule>
@@ -1746,16 +1696,6 @@
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>170</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -1771,13 +1711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43CABD-B29F-401C-947C-ED2BB5BE9B42}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
@@ -1795,20 +1733,20 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1828,7 +1766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1851,7 +1789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -1868,7 +1806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -1883,7 +1821,7 @@
       <c r="F4" s="34"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -1906,7 +1844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -1923,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -1940,7 +1878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -1957,7 +1895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -1974,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -1991,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="36" t="s">
         <v>77</v>
       </c>
@@ -2005,7 +1943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G13">
         <f>SUM(G2:G11)</f>
         <v>34</v>
@@ -2030,16 +1968,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2047,7 +1985,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -2055,7 +1993,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -2081,12 +2019,12 @@
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2102,12 +2040,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
@@ -2128,25 +2066,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" customWidth="1"/>
+    <col min="11" max="11" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="9" t="s">
         <v>39</v>
       </c>
@@ -2156,7 +2094,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
@@ -2178,7 +2116,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
@@ -2202,7 +2140,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>48</v>
       </c>
@@ -2221,7 +2159,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>50</v>
       </c>
@@ -2240,7 +2178,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>52</v>
       </c>
@@ -2260,17 +2198,17 @@
       <c r="H7" s="6"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.7">
       <c r="A9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>55</v>
       </c>
@@ -2282,7 +2220,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>57</v>
       </c>
@@ -2294,7 +2232,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>59</v>
       </c>
@@ -2306,7 +2244,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
@@ -2318,11 +2256,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>62</v>
       </c>
@@ -2334,7 +2272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>63</v>
       </c>
@@ -2346,24 +2284,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:3" ht="31" x14ac:dyDescent="0.7">
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>65</v>
       </c>
@@ -2374,7 +2312,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>52</v>
       </c>
@@ -2383,17 +2321,17 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="10"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:3" ht="31" x14ac:dyDescent="0.7">
       <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>41</v>
       </c>
@@ -2405,7 +2343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>57</v>
       </c>
@@ -2417,7 +2355,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>59</v>
       </c>
@@ -2429,7 +2367,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>61</v>
       </c>
@@ -2441,11 +2379,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>62</v>
       </c>
@@ -2457,7 +2395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
@@ -2469,7 +2407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>

</xml_diff>

<commit_message>
Schematic cleaned up, connectors labeled
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Component_Selection.xlsx
+++ b/00_PROJECT_RESEARCH/Component_Selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CB4E7-81DA-417D-9B6C-4F6958B1895A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5394039E-3BA8-4CF7-B912-C1FBA44AF26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
+    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15370" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Info" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -637,6 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1251,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44782264-4582-4BFB-8AD9-CCF220720B86}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2062,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8DA851-99A2-4738-88A5-6E06B7782D39}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2099,7 +2100,7 @@
         <v>41</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="C3" s="4"/>
       <c r="E3" s="14"/>
@@ -2121,20 +2122,21 @@
         <v>45</v>
       </c>
       <c r="B4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C4" s="4"/>
       <c r="E4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="41">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="27">
         <v>100</v>
       </c>
-      <c r="H4">
-        <v>2</v>
+      <c r="H4" s="41">
+        <f>60*60*F4</f>
+        <v>1.8</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>47</v>
@@ -2151,11 +2153,15 @@
       <c r="E5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="41">
         <v>1E-3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="27">
         <v>100</v>
+      </c>
+      <c r="H5" s="41">
+        <f>30*30*F5</f>
+        <v>0.9</v>
       </c>
       <c r="I5" s="17"/>
     </row>
@@ -2170,11 +2176,15 @@
       <c r="E6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="41">
         <v>2E-3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="27">
         <v>100</v>
+      </c>
+      <c r="H6" s="41">
+        <f>16*16*F6</f>
+        <v>0.51200000000000001</v>
       </c>
       <c r="I6" s="17"/>
     </row>
@@ -2195,7 +2205,10 @@
       <c r="G7" s="6">
         <v>100</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="21">
+        <f>5*5*F7</f>
+        <v>0.16</v>
+      </c>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2214,7 +2227,7 @@
       </c>
       <c r="B10" s="12">
         <f>B12/B3</f>
-        <v>5.3333333333333336E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>56</v>
@@ -2226,7 +2239,7 @@
       </c>
       <c r="B11" s="12">
         <f>B3*B12</f>
-        <v>1.92</v>
+        <v>6.4</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>58</v>
@@ -2250,7 +2263,7 @@
       </c>
       <c r="B13" s="12">
         <f>B4*B10</f>
-        <v>5.3333333333333337E-6</v>
+        <v>1.6E-7</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>60</v>
@@ -2278,7 +2291,7 @@
       </c>
       <c r="B16" s="12">
         <f>B13*B7</f>
-        <v>5.3333333333333336E-4</v>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>60</v>
@@ -2306,7 +2319,7 @@
         <v>65</v>
       </c>
       <c r="B21">
-        <v>5.0000000000000001E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>56</v>
@@ -2337,7 +2350,7 @@
       </c>
       <c r="B25" s="12">
         <f>(B5-B5*(B6/100))/(B21)/B7</f>
-        <v>59.399999999999991</v>
+        <v>148.49999999999997</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>66</v>
@@ -2349,7 +2362,7 @@
       </c>
       <c r="B26" s="12">
         <f>B25*B25*B21</f>
-        <v>1.7641799999999994</v>
+        <v>4.4104499999999991</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>58</v>
@@ -2373,7 +2386,7 @@
       </c>
       <c r="B28" s="12">
         <f>B4*B21</f>
-        <v>5.0000000000000004E-6</v>
+        <v>2.0000000000000002E-7</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>60</v>
@@ -2401,7 +2414,7 @@
       </c>
       <c r="B31" s="12">
         <f>B28*B22</f>
-        <v>5.0000000000000001E-4</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
place 3d model for gigavac
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Component_Selection.xlsx
+++ b/00_PROJECT_RESEARCH/Component_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5394039E-3BA8-4CF7-B912-C1FBA44AF26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DD8ECE-6379-4FFF-AEE8-876610F6EC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15370" tabRatio="671" activeTab="2" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
+    <workbookView xWindow="8020" yWindow="3210" windowWidth="21800" windowHeight="16010" tabRatio="671" activeTab="3" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Info" sheetId="1" r:id="rId1"/>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44782264-4582-4BFB-8AD9-CCF220720B86}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1712,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43CABD-B29F-401C-947C-ED2BB5BE9B42}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>

<commit_message>
spice model for open circuit detection
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Component_Selection.xlsx
+++ b/00_PROJECT_RESEARCH/Component_Selection.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DD8ECE-6379-4FFF-AEE8-876610F6EC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED559B-22E3-4D1D-96D8-BE9AAEAD45BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="3210" windowWidth="21800" windowHeight="16010" tabRatio="671" activeTab="3" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="671" activeTab="4" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Info" sheetId="1" r:id="rId1"/>
     <sheet name="MCU" sheetId="5" r:id="rId2"/>
     <sheet name="MOSFETs" sheetId="3" r:id="rId3"/>
     <sheet name="Gate Drive" sheetId="4" r:id="rId4"/>
-    <sheet name="Connectors" sheetId="2" r:id="rId5"/>
-    <sheet name="Fuses" sheetId="10" r:id="rId6"/>
-    <sheet name="Power Monitors" sheetId="6" r:id="rId7"/>
-    <sheet name="CSA" sheetId="8" r:id="rId8"/>
-    <sheet name="Shunt Resistors" sheetId="7" r:id="rId9"/>
-    <sheet name="Thermals" sheetId="9" r:id="rId10"/>
+    <sheet name="Gigavac" sheetId="11" r:id="rId5"/>
+    <sheet name="Connectors" sheetId="2" r:id="rId6"/>
+    <sheet name="Fuses" sheetId="10" r:id="rId7"/>
+    <sheet name="Power Monitors" sheetId="6" r:id="rId8"/>
+    <sheet name="CSA" sheetId="8" r:id="rId9"/>
+    <sheet name="Shunt Resistors" sheetId="7" r:id="rId10"/>
+    <sheet name="Thermals" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="109">
   <si>
     <t>Current (A)</t>
   </si>
@@ -323,13 +324,64 @@
   </si>
   <si>
     <t>Ambient Cooled (°C/W)</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>GV Normal</t>
+  </si>
+  <si>
+    <t>GV FTDI</t>
+  </si>
+  <si>
+    <t>MOLEX PCBA PINOUT</t>
+  </si>
+  <si>
+    <t>LED ANODE</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>VBATT-</t>
+  </si>
+  <si>
+    <t>VBATT -</t>
+  </si>
+  <si>
+    <t>LED CATHODE / TX to HOST</t>
+  </si>
+  <si>
+    <t>MPUSH-STOP / RX to HOST</t>
+  </si>
+  <si>
+    <t>LED CATHODE</t>
+  </si>
+  <si>
+    <t>TX to HOST</t>
+  </si>
+  <si>
+    <t>MPUSH-START / VBATT+</t>
+  </si>
+  <si>
+    <t>MPUSH-STOP</t>
+  </si>
+  <si>
+    <t>RX to HOST</t>
+  </si>
+  <si>
+    <t>MPUSH-START</t>
+  </si>
+  <si>
+    <t>VBATT+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +434,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -583,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -638,6 +697,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1153,6 +1216,378 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8DA851-99A2-4738-88A5-6E06B7782D39}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" customWidth="1"/>
+    <col min="11" max="11" width="16.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="G2" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="E4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="41">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G4" s="27">
+        <v>100</v>
+      </c>
+      <c r="H4" s="41">
+        <f>60*60*F4</f>
+        <v>1.8</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>3.3</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="41">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="27">
+        <v>100</v>
+      </c>
+      <c r="H5" s="41">
+        <f>30*30*F5</f>
+        <v>0.9</v>
+      </c>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="41">
+        <v>2E-3</v>
+      </c>
+      <c r="G6" s="27">
+        <v>100</v>
+      </c>
+      <c r="H6" s="41">
+        <f>16*16*F6</f>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="E7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="21">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>100</v>
+      </c>
+      <c r="H7" s="21">
+        <f>5*5*F7</f>
+        <v>0.16</v>
+      </c>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.7">
+      <c r="A9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="12">
+        <f>B12/B3</f>
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="12">
+        <f>B3*B12</f>
+        <v>6.4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="12">
+        <f>(B5-B6/100)/B7</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="12">
+        <f>B4*B10</f>
+        <v>1.6E-7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="12">
+        <f>B12*B7</f>
+        <v>3.2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="12">
+        <f>B13*B7</f>
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="31" x14ac:dyDescent="0.7">
+      <c r="A20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="31" x14ac:dyDescent="0.7">
+      <c r="A24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="12">
+        <f>(B5-B5*(B6/100))/(B21)/B7</f>
+        <v>148.49999999999997</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="12">
+        <f>B25*B25*B21</f>
+        <v>4.4104499999999991</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="12">
+        <f>B25*B21</f>
+        <v>2.9699999999999997E-2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="12">
+        <f>B4*B21</f>
+        <v>2.0000000000000002E-7</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="12">
+        <f>B7*B27</f>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="12">
+        <f>B28*B22</f>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A6DD2-EC01-41A2-B284-C1859DA82837}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -1712,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43CABD-B29F-401C-947C-ED2BB5BE9B42}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1730,6 +2165,149 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAF7C8E-8873-4318-8203-B5F6B3F54DCA}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="37">
+        <v>1</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="37">
+        <v>2</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="37">
+        <v>3</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="37">
+        <v>4</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="37">
+        <v>5</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="37">
+        <v>6</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="37">
+        <v>7</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="38"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="37">
+        <v>8</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194B1715-89B1-4EBA-B1B3-6FC5DDCD609A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1964,7 +2542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E847CE7-2AE2-418F-88FE-F3C551DD2CA3}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2012,7 +2590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7C6A1A-F808-46AE-9D0C-CF00964DD3FC}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2035,7 +2613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0616965B-A2B5-49D3-91AA-6EB7CAC3BAA0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2057,376 +2635,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8DA851-99A2-4738-88A5-6E06B7782D39}">
-  <dimension ref="A1:I32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.90625" customWidth="1"/>
-    <col min="10" max="10" width="12.36328125" customWidth="1"/>
-    <col min="11" max="11" width="16.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="G2" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
-        <v>1E-3</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="E4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="41">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G4" s="27">
-        <v>100</v>
-      </c>
-      <c r="H4" s="41">
-        <f>60*60*F4</f>
-        <v>1.8</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5">
-        <v>3.3</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="E5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="41">
-        <v>1E-3</v>
-      </c>
-      <c r="G5" s="27">
-        <v>100</v>
-      </c>
-      <c r="H5" s="41">
-        <f>30*30*F5</f>
-        <v>0.9</v>
-      </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="41">
-        <v>2E-3</v>
-      </c>
-      <c r="G6" s="27">
-        <v>100</v>
-      </c>
-      <c r="H6" s="41">
-        <f>16*16*F6</f>
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="E7" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="21">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="G7" s="6">
-        <v>100</v>
-      </c>
-      <c r="H7" s="21">
-        <f>5*5*F7</f>
-        <v>0.16</v>
-      </c>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.7">
-      <c r="A9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="12">
-        <f>B12/B3</f>
-        <v>1.6000000000000001E-4</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="12">
-        <f>B3*B12</f>
-        <v>6.4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="12">
-        <f>(B5-B6/100)/B7</f>
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="12">
-        <f>B4*B10</f>
-        <v>1.6E-7</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="12">
-        <f>B12*B7</f>
-        <v>3.2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="12">
-        <f>B13*B7</f>
-        <v>1.5999999999999999E-5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31" x14ac:dyDescent="0.7">
-      <c r="A20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22">
-        <v>100</v>
-      </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="31" x14ac:dyDescent="0.7">
-      <c r="A24" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="12">
-        <f>(B5-B5*(B6/100))/(B21)/B7</f>
-        <v>148.49999999999997</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="12">
-        <f>B25*B25*B21</f>
-        <v>4.4104499999999991</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="12">
-        <f>B25*B21</f>
-        <v>2.9699999999999997E-2</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="12">
-        <f>B4*B21</f>
-        <v>2.0000000000000002E-7</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="12">
-        <f>B7*B27</f>
-        <v>2.9699999999999998</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="12">
-        <f>B28*B22</f>
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx sheet with micro pin maps
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Component_Selection.xlsx
+++ b/00_PROJECT_RESEARCH/Component_Selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96713AE4-B7A5-4467-907D-44BFBB8EEE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0E4271-38E4-465A-9794-AB94770EE1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="671" activeTab="1" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
@@ -1832,7 +1832,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:F32"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>